<commit_message>
modif commentaire et plan test acceptation
</commit_message>
<xml_diff>
--- a/Plan tests d'acceptation.xlsx
+++ b/Plan tests d'acceptation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -85,9 +85,6 @@
     <t>methode fetch() lancé dès la page d'accueil se charge</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>Affichage de l'ensemble des produits sur la page d'accueil</t>
   </si>
   <si>
@@ -154,20 +151,77 @@
     <t>Envoyer le formulaire</t>
   </si>
   <si>
-    <t>Envoi du formulaire et de toutes les données au back end</t>
-  </si>
-  <si>
     <t>Cliquer sur le bouton "commander" et l'envoi s'effectu grâce à la méthode POST fetch()</t>
   </si>
   <si>
     <t xml:space="preserve">Insérer les caractères dans le formulaire au bon endroit </t>
+  </si>
+  <si>
+    <t>Légende des couleurs correspondant aux différents script JS</t>
+  </si>
+  <si>
+    <t>Script.js</t>
+  </si>
+  <si>
+    <t>Product.js</t>
+  </si>
+  <si>
+    <t>Cart.js</t>
+  </si>
+  <si>
+    <t>Confirmation.js</t>
+  </si>
+  <si>
+    <t>OK / Aucune images affichées</t>
+  </si>
+  <si>
+    <t>OK / Affichage du mauvais produit</t>
+  </si>
+  <si>
+    <t>OK / Aucun produit affiché</t>
+  </si>
+  <si>
+    <t>OK / Le produit n'est pas le bon ou rien ne s'affiche</t>
+  </si>
+  <si>
+    <t>OK / Mauvaise couleur ou quantité affichée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK / Produit pas stocké </t>
+  </si>
+  <si>
+    <t>OK / Les éléments ne s'actualisent pas lors du changement de couleurs ou quantité</t>
+  </si>
+  <si>
+    <t>OK / Les produits ne s'affichent pas sur la page panier</t>
+  </si>
+  <si>
+    <t>OK /  Le produit rentre en conflit avec celui comportant le même ID</t>
+  </si>
+  <si>
+    <t>OK / Les éléments ne s'actualisent pas lors de la modifcations du produit</t>
+  </si>
+  <si>
+    <t>Envoi du formulaire et de toutes les données au back end en supprimant le localStorage</t>
+  </si>
+  <si>
+    <t>OK / Le formulaire est envoyé mais le localStorage n'est pas supprimé ou les donnée ne sont pas correctement envoyé au back end</t>
+  </si>
+  <si>
+    <t>OK / Le numéro de la commande n'est pas affiché ou ne correspond pas</t>
+  </si>
+  <si>
+    <t>OK / Informations incorrects le formulaire ne s'envoient pas et montre l'endroit ou il y a un erreur avec un message en dessous</t>
+  </si>
+  <si>
+    <t>OK / Le produit reste affiché ou reste stocké</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -187,6 +241,20 @@
     <font>
       <sz val="14"/>
       <name val="Montserrat"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -227,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -446,11 +514,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -522,6 +605,23 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -734,10 +834,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -774,10 +874,10 @@
         <v>22</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54">
@@ -791,7 +891,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>6</v>
@@ -802,16 +902,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" s="12" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="54">
@@ -822,13 +922,13 @@
         <v>21</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="54">
@@ -839,13 +939,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="54">
@@ -862,7 +962,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36">
@@ -876,10 +976,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36">
@@ -887,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>14</v>
@@ -896,7 +996,7 @@
         <v>15</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36">
@@ -904,16 +1004,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>39</v>
-      </c>
       <c r="E10" s="21" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="54">
@@ -927,10 +1027,10 @@
         <v>17</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="54">
@@ -938,16 +1038,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="36">
@@ -961,10 +1061,10 @@
         <v>19</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="72">
@@ -972,33 +1072,33 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="36">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="72">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>47</v>
-      </c>
       <c r="D15" s="20" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="36.75" thickBot="1">
@@ -1009,13 +1109,42 @@
         <v>20</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>23</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A18" s="25"/>
+      <c r="B18" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A19" s="25"/>
+      <c r="B19" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A20" s="25"/>
+      <c r="B20" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A21" s="26"/>
+      <c r="B21" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="45.6" customHeight="1">
+      <c r="B23" s="27" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>